<commit_message>
#25 Added methods for converting XlBean values to primitive types
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/TestBook_XlBean.xlsx
+++ b/src/test/resources/org/xlbean/TestBook_XlBean.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01672BE5-4797-408F-B5DD-E325141AF94D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8230" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="int" sheetId="6" r:id="rId2"/>
+    <sheet name="long" sheetId="7" r:id="rId3"/>
+    <sheet name="short" sheetId="8" r:id="rId4"/>
+    <sheet name="float" sheetId="9" r:id="rId5"/>
+    <sheet name="double" sheetId="10" r:id="rId6"/>
+    <sheet name="bool" sheetId="11" r:id="rId7"/>
+    <sheet name="char" sheetId="12" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="173">
   <si>
     <t>####</t>
     <phoneticPr fontId="1"/>
@@ -307,6 +315,341 @@
   </si>
   <si>
     <t>extract#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>int4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>last</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>error1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>error2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>props#key?listToProp=key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ints[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>props#~</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ints[1]</t>
+  </si>
+  <si>
+    <t>ints[2]</t>
+  </si>
+  <si>
+    <t>ints[3]</t>
+  </si>
+  <si>
+    <t>ints[4]</t>
+  </si>
+  <si>
+    <t>ints[5]</t>
+  </si>
+  <si>
+    <t>ints[6]</t>
+  </si>
+  <si>
+    <t>props#value?listToProp=value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>long1</t>
+  </si>
+  <si>
+    <t>long2</t>
+  </si>
+  <si>
+    <t>long3</t>
+  </si>
+  <si>
+    <t>long4</t>
+  </si>
+  <si>
+    <t>longs[0]</t>
+  </si>
+  <si>
+    <t>longs[1]</t>
+  </si>
+  <si>
+    <t>longs[2]</t>
+  </si>
+  <si>
+    <t>longs[3]</t>
+  </si>
+  <si>
+    <t>longs[4]</t>
+  </si>
+  <si>
+    <t>longs[5]</t>
+  </si>
+  <si>
+    <t>longs[6]</t>
+  </si>
+  <si>
+    <t>long5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9223372036854775807</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>longs[7]</t>
+  </si>
+  <si>
+    <t>short1</t>
+  </si>
+  <si>
+    <t>short2</t>
+  </si>
+  <si>
+    <t>short3</t>
+  </si>
+  <si>
+    <t>short4</t>
+  </si>
+  <si>
+    <t>short5</t>
+  </si>
+  <si>
+    <t>shorts[0]</t>
+  </si>
+  <si>
+    <t>shorts[1]</t>
+  </si>
+  <si>
+    <t>shorts[2]</t>
+  </si>
+  <si>
+    <t>shorts[3]</t>
+  </si>
+  <si>
+    <t>shorts[4]</t>
+  </si>
+  <si>
+    <t>shorts[5]</t>
+  </si>
+  <si>
+    <t>shorts[6]</t>
+  </si>
+  <si>
+    <t>shorts[7]</t>
+  </si>
+  <si>
+    <t>float1</t>
+  </si>
+  <si>
+    <t>float2</t>
+  </si>
+  <si>
+    <t>float3</t>
+  </si>
+  <si>
+    <t>float4</t>
+  </si>
+  <si>
+    <t>float5</t>
+  </si>
+  <si>
+    <t>floats[0]</t>
+  </si>
+  <si>
+    <t>floats[1]</t>
+  </si>
+  <si>
+    <t>floats[2]</t>
+  </si>
+  <si>
+    <t>floats[3]</t>
+  </si>
+  <si>
+    <t>floats[4]</t>
+  </si>
+  <si>
+    <t>floats[5]</t>
+  </si>
+  <si>
+    <t>floats[6]</t>
+  </si>
+  <si>
+    <t>floats[7]</t>
+  </si>
+  <si>
+    <t>double1</t>
+  </si>
+  <si>
+    <t>double2</t>
+  </si>
+  <si>
+    <t>double3</t>
+  </si>
+  <si>
+    <t>double4</t>
+  </si>
+  <si>
+    <t>double5</t>
+  </si>
+  <si>
+    <t>doubles[0]</t>
+  </si>
+  <si>
+    <t>doubles[1]</t>
+  </si>
+  <si>
+    <t>doubles[2]</t>
+  </si>
+  <si>
+    <t>doubles[3]</t>
+  </si>
+  <si>
+    <t>doubles[4]</t>
+  </si>
+  <si>
+    <t>doubles[5]</t>
+  </si>
+  <si>
+    <t>doubles[6]</t>
+  </si>
+  <si>
+    <t>doubles[7]</t>
+  </si>
+  <si>
+    <t>bool1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bool2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bool3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TRUE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bool4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>falSE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>true1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bools[0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bools[1]</t>
+  </si>
+  <si>
+    <t>bools[2]</t>
+  </si>
+  <si>
+    <t>bools[3]</t>
+  </si>
+  <si>
+    <t>bools[4]</t>
+  </si>
+  <si>
+    <t>bools[5]</t>
+  </si>
+  <si>
+    <t>bools[6]</t>
+  </si>
+  <si>
+    <t>bool5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bool_error1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bool_error2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>character1</t>
+  </si>
+  <si>
+    <t>character2</t>
+  </si>
+  <si>
+    <t>character3</t>
+  </si>
+  <si>
+    <t>character4</t>
+  </si>
+  <si>
+    <t>characters[0]</t>
+  </si>
+  <si>
+    <t>characters[1]</t>
+  </si>
+  <si>
+    <t>characters[2]</t>
+  </si>
+  <si>
+    <t>characters[3]</t>
+  </si>
+  <si>
+    <t>characters[4]</t>
+  </si>
+  <si>
+    <t>characters[5]</t>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bcde111</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>character5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>character6</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -353,11 +696,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -676,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A66886-8370-47E9-9AD6-6A526655F5D9}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -1417,4 +1763,1051 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57882E8F-0D14-4C43-AC14-C5F870161CEA}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7647D-D14A-4D95-B1ED-99FEC201BE25}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D2BB03-2200-49DD-A534-D17054F37120}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6747E0D-53E3-46E0-8B8D-DCAEC3F0FA01}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2875F5DF-86A2-40D8-AF87-CE4814C15BC1}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42FE039-8EA6-4C11-ADC4-1E7E796269EA}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649CDD1E-3590-4813-8A22-CFBB3F051641}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.9140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" s="2">
+        <v>-1234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#48 Changed toBean to toMap
</commit_message>
<xml_diff>
--- a/src/test/resources/org/xlbean/TestBook_XlBean.xlsx
+++ b/src/test/resources/org/xlbean/TestBook_XlBean.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanikawa\git\xlbean\src\test\resources\org\xlbean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C816B23-64EA-4C68-A48A-81B99FB44FCC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106E71C9-83CA-47E2-A406-D31D1EB7E9CA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8712" yWindow="0" windowWidth="19200" windowHeight="8232" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="1044" windowWidth="21948" windowHeight="12660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -700,10 +700,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>props#key?toBean=key</t>
-  </si>
-  <si>
-    <t>props#value?toBean=value</t>
+    <t>props#key?toMap=key</t>
+  </si>
+  <si>
+    <t>props#value?toMap=value</t>
   </si>
 </sst>
 </file>

</xml_diff>